<commit_message>
Correct stochastoic SEIR results and plots!
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSEIR_Scenario0_Primer_200_gamma.xlsx
+++ b/results/primer/VanillaSEIR_Scenario0_Primer_200_gamma.xlsx
@@ -450,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI1"/>
+  <dimension ref="A1:AI6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -563,6 +563,541 @@
         <v>34</v>
       </c>
     </row>
+    <row r="2" spans="1:35">
+      <c r="A2">
+        <v>0.3300368681588889</v>
+      </c>
+      <c r="B2">
+        <v>0.295472258886636</v>
+      </c>
+      <c r="C2">
+        <v>0.3631211525990467</v>
+      </c>
+      <c r="D2">
+        <v>0.2722860630512539</v>
+      </c>
+      <c r="E2">
+        <v>0.4068499506284093</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+      <c r="P2">
+        <v>2.310258077112223</v>
+      </c>
+      <c r="Q2">
+        <v>2.068305812206452</v>
+      </c>
+      <c r="R2">
+        <v>2.541848068193326</v>
+      </c>
+      <c r="S2">
+        <v>1.906002441358778</v>
+      </c>
+      <c r="T2">
+        <v>2.847949654398865</v>
+      </c>
+      <c r="U2">
+        <v>100.58425</v>
+      </c>
+      <c r="V2">
+        <v>87.68037383032676</v>
+      </c>
+      <c r="W2">
+        <v>112.350909364063</v>
+      </c>
+      <c r="X2">
+        <v>77.78486367272372</v>
+      </c>
+      <c r="Y2">
+        <v>128.7766997559584</v>
+      </c>
+      <c r="Z2">
+        <v>0.127699338494011</v>
+      </c>
+      <c r="AA2">
+        <v>0.1038513871225602</v>
+      </c>
+      <c r="AB2">
+        <v>0.151622640529654</v>
+      </c>
+      <c r="AC2">
+        <v>0.08604351479746133</v>
+      </c>
+      <c r="AD2">
+        <v>0.1749317536996756</v>
+      </c>
+      <c r="AE2">
+        <v>0.8571964331914291</v>
+      </c>
+      <c r="AF2">
+        <v>0.8112199873047428</v>
+      </c>
+      <c r="AG2">
+        <v>0.8979354764039813</v>
+      </c>
+      <c r="AH2">
+        <v>0.7705929268849784</v>
+      </c>
+      <c r="AI2">
+        <v>0.9301073959422517</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35">
+      <c r="A3">
+        <v>0.33</v>
+      </c>
+      <c r="B3">
+        <v>0.33</v>
+      </c>
+      <c r="C3">
+        <v>0.33</v>
+      </c>
+      <c r="D3">
+        <v>0.33</v>
+      </c>
+      <c r="E3">
+        <v>0.33</v>
+      </c>
+      <c r="F3">
+        <v>6.997208238996328</v>
+      </c>
+      <c r="G3">
+        <v>6.211708480501438</v>
+      </c>
+      <c r="H3">
+        <v>7.750615725360402</v>
+      </c>
+      <c r="I3">
+        <v>5.697852097493597</v>
+      </c>
+      <c r="J3">
+        <v>8.761324523328691</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <v>2.309078718868789</v>
+      </c>
+      <c r="Q3">
+        <v>2.049863798565474</v>
+      </c>
+      <c r="R3">
+        <v>2.557703189368933</v>
+      </c>
+      <c r="S3">
+        <v>1.880291192172887</v>
+      </c>
+      <c r="T3">
+        <v>2.891237092698468</v>
+      </c>
+      <c r="U3">
+        <v>99.94318</v>
+      </c>
+      <c r="V3">
+        <v>92.74969224531547</v>
+      </c>
+      <c r="W3">
+        <v>107.3669139784783</v>
+      </c>
+      <c r="X3">
+        <v>87.51808929487457</v>
+      </c>
+      <c r="Y3">
+        <v>115.0151989085309</v>
+      </c>
+      <c r="Z3">
+        <v>0.1280655974290327</v>
+      </c>
+      <c r="AA3">
+        <v>0.09771137674306317</v>
+      </c>
+      <c r="AB3">
+        <v>0.1597094549971312</v>
+      </c>
+      <c r="AC3">
+        <v>0.07615470438817838</v>
+      </c>
+      <c r="AD3">
+        <v>0.1925575142439491</v>
+      </c>
+      <c r="AE3">
+        <v>0.8559038826910592</v>
+      </c>
+      <c r="AF3">
+        <v>0.806321355153669</v>
+      </c>
+      <c r="AG3">
+        <v>0.8998248219988605</v>
+      </c>
+      <c r="AH3">
+        <v>0.7628449515139616</v>
+      </c>
+      <c r="AI3">
+        <v>0.9340592150328463</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35">
+      <c r="A4">
+        <v>0.3299546669000036</v>
+      </c>
+      <c r="B4">
+        <v>0.2954865006110795</v>
+      </c>
+      <c r="C4">
+        <v>0.3628830664704524</v>
+      </c>
+      <c r="D4">
+        <v>0.2720329806800469</v>
+      </c>
+      <c r="E4">
+        <v>0.407098622037785</v>
+      </c>
+      <c r="F4">
+        <v>6.99827874932453</v>
+      </c>
+      <c r="G4">
+        <v>6.211970424988903</v>
+      </c>
+      <c r="H4">
+        <v>7.745037165329355</v>
+      </c>
+      <c r="I4">
+        <v>5.701645464256834</v>
+      </c>
+      <c r="J4">
+        <v>8.770715711799282</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <v>2.309030454651602</v>
+      </c>
+      <c r="Q4">
+        <v>1.957856982297311</v>
+      </c>
+      <c r="R4">
+        <v>2.64493494335285</v>
+      </c>
+      <c r="S4">
+        <v>1.725062703407883</v>
+      </c>
+      <c r="T4">
+        <v>3.108858007767917</v>
+      </c>
+      <c r="U4">
+        <v>102.08827</v>
+      </c>
+      <c r="V4">
+        <v>87.09196012881102</v>
+      </c>
+      <c r="W4">
+        <v>116.5183351204225</v>
+      </c>
+      <c r="X4">
+        <v>76.61988320651332</v>
+      </c>
+      <c r="Y4">
+        <v>138.3072911618482</v>
+      </c>
+      <c r="Z4">
+        <v>0.127053027103331</v>
+      </c>
+      <c r="AA4">
+        <v>0.08886379706095983</v>
+      </c>
+      <c r="AB4">
+        <v>0.1661520603053158</v>
+      </c>
+      <c r="AC4">
+        <v>0.06100639498027485</v>
+      </c>
+      <c r="AD4">
+        <v>0.2056703573250038</v>
+      </c>
+      <c r="AE4">
+        <v>0.8487558790433356</v>
+      </c>
+      <c r="AF4">
+        <v>0.7772784448030349</v>
+      </c>
+      <c r="AG4">
+        <v>0.9078315424462871</v>
+      </c>
+      <c r="AH4">
+        <v>0.7061324731648092</v>
+      </c>
+      <c r="AI4">
+        <v>0.9513991009616451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35">
+      <c r="A5">
+        <v>0.33</v>
+      </c>
+      <c r="B5">
+        <v>0.33</v>
+      </c>
+      <c r="C5">
+        <v>0.33</v>
+      </c>
+      <c r="D5">
+        <v>0.33</v>
+      </c>
+      <c r="E5">
+        <v>0.33</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
+      <c r="K5">
+        <v>3.99890249252565</v>
+      </c>
+      <c r="L5">
+        <v>3.54783857102002</v>
+      </c>
+      <c r="M5">
+        <v>4.431856646837604</v>
+      </c>
+      <c r="N5">
+        <v>3.165981920593907</v>
+      </c>
+      <c r="O5">
+        <v>4.927173857001854</v>
+      </c>
+      <c r="P5">
+        <v>2.31</v>
+      </c>
+      <c r="Q5">
+        <v>2.31</v>
+      </c>
+      <c r="R5">
+        <v>2.31</v>
+      </c>
+      <c r="S5">
+        <v>2.31</v>
+      </c>
+      <c r="T5">
+        <v>2.31</v>
+      </c>
+      <c r="U5">
+        <v>98.52849000000001</v>
+      </c>
+      <c r="V5">
+        <v>93.79558246075284</v>
+      </c>
+      <c r="W5">
+        <v>103.1431825745692</v>
+      </c>
+      <c r="X5">
+        <v>89.93686124676002</v>
+      </c>
+      <c r="Y5">
+        <v>107.6585286999046</v>
+      </c>
+      <c r="Z5">
+        <v>0.1289788574428249</v>
+      </c>
+      <c r="AA5">
+        <v>0.1233500633980511</v>
+      </c>
+      <c r="AB5">
+        <v>0.1343574825850218</v>
+      </c>
+      <c r="AC5">
+        <v>0.1186524547236349</v>
+      </c>
+      <c r="AD5">
+        <v>0.1394438571624682</v>
+      </c>
+      <c r="AE5">
+        <v>0.86416766455395</v>
+      </c>
+      <c r="AF5">
+        <v>0.8641670458907781</v>
+      </c>
+      <c r="AG5">
+        <v>0.8641680178366636</v>
+      </c>
+      <c r="AH5">
+        <v>0.8641659827486737</v>
+      </c>
+      <c r="AI5">
+        <v>0.8641683396216523</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35">
+      <c r="A6">
+        <v>0.33002046411242</v>
+      </c>
+      <c r="B6">
+        <v>0.2953763363915379</v>
+      </c>
+      <c r="C6">
+        <v>0.3632716599738005</v>
+      </c>
+      <c r="D6">
+        <v>0.2718840422252982</v>
+      </c>
+      <c r="E6">
+        <v>0.4065125934875387</v>
+      </c>
+      <c r="F6">
+        <v>6.998500463445088</v>
+      </c>
+      <c r="G6">
+        <v>6.209881634710266</v>
+      </c>
+      <c r="H6">
+        <v>7.756141471337187</v>
+      </c>
+      <c r="I6">
+        <v>5.698366000827131</v>
+      </c>
+      <c r="J6">
+        <v>8.768556060092456</v>
+      </c>
+      <c r="K6">
+        <v>3.999545593737989</v>
+      </c>
+      <c r="L6">
+        <v>3.548838938696382</v>
+      </c>
+      <c r="M6">
+        <v>4.432336156891433</v>
+      </c>
+      <c r="N6">
+        <v>3.172164494650679</v>
+      </c>
+      <c r="O6">
+        <v>4.920191628817671</v>
+      </c>
+      <c r="P6">
+        <v>2.309632089802328</v>
+      </c>
+      <c r="Q6">
+        <v>1.957416985369304</v>
+      </c>
+      <c r="R6">
+        <v>2.647699099948058</v>
+      </c>
+      <c r="S6">
+        <v>1.721622927877045</v>
+      </c>
+      <c r="T6">
+        <v>3.111835247514327</v>
+      </c>
+      <c r="U6">
+        <v>102.04347</v>
+      </c>
+      <c r="V6">
+        <v>86.25076848911166</v>
+      </c>
+      <c r="W6">
+        <v>116.9307385069291</v>
+      </c>
+      <c r="X6">
+        <v>75.21182886888346</v>
+      </c>
+      <c r="Y6">
+        <v>138.7914045077047</v>
+      </c>
+      <c r="Z6">
+        <v>0.1273154517357958</v>
+      </c>
+      <c r="AA6">
+        <v>0.08857550152371189</v>
+      </c>
+      <c r="AB6">
+        <v>0.1670925343653169</v>
+      </c>
+      <c r="AC6">
+        <v>0.0603878923248169</v>
+      </c>
+      <c r="AD6">
+        <v>0.207527434219609</v>
+      </c>
+      <c r="AE6">
+        <v>0.8486599693161534</v>
+      </c>
+      <c r="AF6">
+        <v>0.7767003830988098</v>
+      </c>
+      <c r="AG6">
+        <v>0.9080318014720987</v>
+      </c>
+      <c r="AH6">
+        <v>0.7047214527548993</v>
+      </c>
+      <c r="AI6">
+        <v>0.9519399972407894</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>